<commit_message>
leetcode pandas introduction practice
</commit_message>
<xml_diff>
--- a/general_practice.xlsx
+++ b/general_practice.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajnish/Projects/Data Engineering/leetcode_pandas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9B51EB-FA67-7947-8134-0CDBAC5A0AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78E9DE4-784A-5C4F-9495-F1597407FD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="20120" windowHeight="16140" activeTab="2" xr2:uid="{125E4D3A-6135-FF45-A452-AE7DCD245EBB}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="20120" windowHeight="16140" activeTab="3" xr2:uid="{125E4D3A-6135-FF45-A452-AE7DCD245EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="players" sheetId="1" r:id="rId1"/>
     <sheet name="employees" sheetId="3" r:id="rId2"/>
     <sheet name="students" sheetId="4" r:id="rId3"/>
-    <sheet name="customers" sheetId="5" r:id="rId4"/>
+    <sheet name="products" sheetId="7" r:id="rId4"/>
+    <sheet name="new_students" sheetId="6" r:id="rId5"/>
+    <sheet name="customers" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
     <t>player_id</t>
   </si>
@@ -231,12 +233,63 @@
   </si>
   <si>
     <t>Willow</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>Wright</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Hall</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>grades</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Wristwatch</t>
+  </si>
+  <si>
+    <t>WirelessEarbuds</t>
+  </si>
+  <si>
+    <t>GolfClubs</t>
+  </si>
+  <si>
+    <t>Printer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -273,9 +326,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,15 +992,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F75880DE-83D3-4D43-A42E-29D383A32FAD}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -956,8 +1013,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>101</v>
       </c>
@@ -967,8 +1027,11 @@
       <c r="C2">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>53</v>
       </c>
@@ -978,8 +1041,11 @@
       <c r="C3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>128</v>
       </c>
@@ -989,8 +1055,11 @@
       <c r="C4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1000,8 +1069,11 @@
       <c r="C5">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>32</v>
       </c>
@@ -1011,8 +1083,11 @@
       <c r="C6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>217</v>
       </c>
@@ -1022,8 +1097,11 @@
       <c r="C7">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>779</v>
       </c>
@@ -1033,8 +1111,11 @@
       <c r="C8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>849</v>
       </c>
@@ -1043,6 +1124,9 @@
       </c>
       <c r="C9">
         <v>14</v>
+      </c>
+      <c r="D9" s="2">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1051,11 +1135,179 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44E3304-08D8-7D48-ABAA-0181BD1EE889}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <v>779</v>
+      </c>
+      <c r="C4">
+        <v>9319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5">
+        <v>849</v>
+      </c>
+      <c r="C5">
+        <v>3051</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D2C36D-77D7-904C-8730-C6C13222D3D3}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4240844B-F18C-774F-BCCA-CC29CEF2097D}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>